<commit_message>
Trabalhando no objeto segurado
</commit_message>
<xml_diff>
--- a/Docs/Acompanhamento da Sprint/Status do backlog.xlsx
+++ b/Docs/Acompanhamento da Sprint/Status do backlog.xlsx
@@ -1,8 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\projetos\seguradora\Docs\Acompanhamento da Sprint\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="240" yWindow="30" windowWidth="20115" windowHeight="8010"/>
   </bookViews>
@@ -16,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
   <si>
     <t>Prioridade</t>
   </si>
@@ -73,13 +78,19 @@
   </si>
   <si>
     <t>Ricardo</t>
+  </si>
+  <si>
+    <t>Leandro</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Desenvolvendo </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="3">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -341,7 +352,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -351,6 +362,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -378,15 +392,21 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -433,7 +453,7 @@
     </a:clrScheme>
     <a:fontScheme name="Escritório">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -465,9 +485,10 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -499,6 +520,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Escritório">
@@ -674,14 +696,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F21"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H5" sqref="H5"/>
+      <selection activeCell="G16" sqref="G16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="10.28515625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="34" bestFit="1" customWidth="1"/>
@@ -689,7 +711,7 @@
     <col min="5" max="5" width="15" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -702,14 +724,14 @@
       <c r="D1" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="E1" s="18" t="s">
+      <c r="E1" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="F1" s="18" t="s">
+      <c r="F1" s="9" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:6">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="5">
         <v>1</v>
       </c>
@@ -719,13 +741,13 @@
       <c r="C2" s="1">
         <v>1</v>
       </c>
-      <c r="D2" s="19">
+      <c r="D2" s="10">
         <v>79</v>
       </c>
       <c r="E2" s="1"/>
       <c r="F2" s="1"/>
     </row>
-    <row r="3" spans="1:6">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="5">
         <v>2</v>
       </c>
@@ -735,13 +757,13 @@
       <c r="C3" s="1">
         <v>2</v>
       </c>
-      <c r="D3" s="19">
+      <c r="D3" s="10">
         <v>39</v>
       </c>
       <c r="E3" s="1"/>
       <c r="F3" s="1"/>
     </row>
-    <row r="4" spans="1:6">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="5">
         <v>2</v>
       </c>
@@ -751,13 +773,13 @@
       <c r="C4" s="1">
         <v>2</v>
       </c>
-      <c r="D4" s="19">
+      <c r="D4" s="10">
         <v>39</v>
       </c>
       <c r="E4" s="1"/>
       <c r="F4" s="1"/>
     </row>
-    <row r="5" spans="1:6">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="5">
         <v>1</v>
       </c>
@@ -767,7 +789,7 @@
       <c r="C5" s="1">
         <v>1</v>
       </c>
-      <c r="D5" s="19">
+      <c r="D5" s="10">
         <v>79</v>
       </c>
       <c r="E5" s="1" t="s">
@@ -777,7 +799,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="6" spans="1:6">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="5">
         <v>1</v>
       </c>
@@ -787,13 +809,17 @@
       <c r="C6" s="1">
         <v>1</v>
       </c>
-      <c r="D6" s="19">
+      <c r="D6" s="10">
         <v>79</v>
       </c>
-      <c r="E6" s="1"/>
-      <c r="F6" s="1"/>
-    </row>
-    <row r="7" spans="1:6">
+      <c r="E6" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="5">
         <v>2</v>
       </c>
@@ -803,13 +829,13 @@
       <c r="C7" s="1">
         <v>1</v>
       </c>
-      <c r="D7" s="19">
+      <c r="D7" s="10">
         <v>79</v>
       </c>
       <c r="E7" s="1"/>
       <c r="F7" s="1"/>
     </row>
-    <row r="8" spans="1:6">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="5">
         <v>2</v>
       </c>
@@ -819,13 +845,13 @@
       <c r="C8" s="1">
         <v>2</v>
       </c>
-      <c r="D8" s="19">
+      <c r="D8" s="10">
         <v>79</v>
       </c>
       <c r="E8" s="1"/>
       <c r="F8" s="1"/>
     </row>
-    <row r="9" spans="1:6">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="5">
         <v>3</v>
       </c>
@@ -835,13 +861,13 @@
       <c r="C9" s="1">
         <v>2</v>
       </c>
-      <c r="D9" s="19">
+      <c r="D9" s="10">
         <v>79</v>
       </c>
       <c r="E9" s="1"/>
       <c r="F9" s="1"/>
     </row>
-    <row r="10" spans="1:6">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="5">
         <v>3</v>
       </c>
@@ -851,13 +877,13 @@
       <c r="C10" s="1">
         <v>3</v>
       </c>
-      <c r="D10" s="19">
+      <c r="D10" s="10">
         <v>39</v>
       </c>
       <c r="E10" s="1"/>
       <c r="F10" s="1"/>
     </row>
-    <row r="11" spans="1:6" ht="15.75" thickBot="1">
+    <row r="11" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="6">
         <v>3</v>
       </c>
@@ -867,69 +893,70 @@
       <c r="C11" s="7">
         <v>3</v>
       </c>
-      <c r="D11" s="20">
+      <c r="D11" s="11">
         <v>39</v>
       </c>
       <c r="E11" s="1"/>
       <c r="F11" s="1"/>
     </row>
-    <row r="12" spans="1:6" ht="15.75" thickBot="1"/>
-    <row r="13" spans="1:6">
-      <c r="A13" s="9" t="s">
+    <row r="12" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A13" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="B13" s="10"/>
-      <c r="C13" s="10"/>
-      <c r="D13" s="11"/>
+      <c r="B13" s="13"/>
+      <c r="C13" s="13"/>
+      <c r="D13" s="14"/>
       <c r="E13" s="8"/>
     </row>
-    <row r="14" spans="1:6">
-      <c r="A14" s="12"/>
-      <c r="B14" s="13"/>
-      <c r="C14" s="13"/>
-      <c r="D14" s="14"/>
-    </row>
-    <row r="15" spans="1:6">
-      <c r="A15" s="12"/>
-      <c r="B15" s="13"/>
-      <c r="C15" s="13"/>
-      <c r="D15" s="14"/>
-    </row>
-    <row r="16" spans="1:6">
-      <c r="A16" s="12"/>
-      <c r="B16" s="13"/>
-      <c r="C16" s="13"/>
-      <c r="D16" s="14"/>
-    </row>
-    <row r="17" spans="1:4">
-      <c r="A17" s="12"/>
-      <c r="B17" s="13"/>
-      <c r="C17" s="13"/>
-      <c r="D17" s="14"/>
-    </row>
-    <row r="18" spans="1:4">
-      <c r="A18" s="12"/>
-      <c r="B18" s="13"/>
-      <c r="C18" s="13"/>
-      <c r="D18" s="14"/>
-    </row>
-    <row r="19" spans="1:4">
-      <c r="A19" s="12"/>
-      <c r="B19" s="13"/>
-      <c r="C19" s="13"/>
-      <c r="D19" s="14"/>
-    </row>
-    <row r="20" spans="1:4">
-      <c r="A20" s="12"/>
-      <c r="B20" s="13"/>
-      <c r="C20" s="13"/>
-      <c r="D20" s="14"/>
-    </row>
-    <row r="21" spans="1:4" ht="15.75" thickBot="1">
-      <c r="A21" s="15"/>
-      <c r="B21" s="16"/>
-      <c r="C21" s="16"/>
-      <c r="D21" s="17"/>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A14" s="15"/>
+      <c r="B14" s="16"/>
+      <c r="C14" s="16"/>
+      <c r="D14" s="17"/>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A15" s="15"/>
+      <c r="B15" s="16"/>
+      <c r="C15" s="16"/>
+      <c r="D15" s="17"/>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A16" s="15"/>
+      <c r="B16" s="16"/>
+      <c r="C16" s="16"/>
+      <c r="D16" s="17"/>
+      <c r="G16" s="21"/>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" s="15"/>
+      <c r="B17" s="16"/>
+      <c r="C17" s="16"/>
+      <c r="D17" s="17"/>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18" s="15"/>
+      <c r="B18" s="16"/>
+      <c r="C18" s="16"/>
+      <c r="D18" s="17"/>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19" s="15"/>
+      <c r="B19" s="16"/>
+      <c r="C19" s="16"/>
+      <c r="D19" s="17"/>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20" s="15"/>
+      <c r="B20" s="16"/>
+      <c r="C20" s="16"/>
+      <c r="D20" s="17"/>
+    </row>
+    <row r="21" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="18"/>
+      <c r="B21" s="19"/>
+      <c r="C21" s="19"/>
+      <c r="D21" s="20"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -941,24 +968,24 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
 </worksheet>

</xml_diff>